<commit_message>
Added Share of AS
Added a Chart for Share of Accumulated Suspects (Accumulated Confirmed, Accumulated Negatives, Accumulated Pending Labs). Helps to understand the evolution of the share of Positive (Confirmed) Cases from the total accumulated number of Suspects (which equals the number of tests performed).
</commit_message>
<xml_diff>
--- a/COVID19 PT.xlsx
+++ b/COVID19 PT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miami\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944EB1AA-AC1C-4700-83C3-F54E281E1F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009639DF-E74A-4BCC-86F8-54851798F061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="8" xr2:uid="{690E66F5-A47F-45E5-A75B-442D4617D3F3}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="9" xr2:uid="{690E66F5-A47F-45E5-A75B-442D4617D3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="FCT DNC 28" sheetId="13" r:id="rId7"/>
     <sheet name="Evolution" sheetId="7" r:id="rId8"/>
     <sheet name="RoG" sheetId="18" r:id="rId9"/>
+    <sheet name="Share AS" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -257,6 +258,9 @@
   </si>
   <si>
     <t>Weekday % DNV</t>
+  </si>
+  <si>
+    <t>AN % AS</t>
   </si>
 </sst>
 </file>
@@ -692,7 +696,49 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="67">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Arial Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
@@ -9666,6 +9712,1027 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Share % of AS</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (AC, AL &amp; AN)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AA$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AC % AS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mm/yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>43887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43897</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43900</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43902</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43920</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AA$2:$AA$35</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3529411764705882E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9603960396039604E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.128205128205128E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1224489795918366E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.18232044198895E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.10676156583629894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11504424778761062</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.10933333333333334</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12526539278131635</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.12244897959183673</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5626911314984705E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.9178403755868547E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.10788199031263761</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.11382393397524071</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.11116625310173697</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.12670219064535229</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.12951658142220757</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.13191929643041903</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.12989648873553886</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.13583496052296459</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.150650870264736</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.1526431433372108</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.14157409595840226</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.15923080379206542</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.16782666823955014</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.15784331684679734</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2478-4672-B213-1EA7FF9603CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AG$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AL % AS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mm/yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>43887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43897</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43900</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43902</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43920</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AG$2:$AG$35</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16574585635359115</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20982142857142858</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.199288256227758</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.19764011799410031</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22133333333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17622080679405519</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2087912087912088</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.13149847094801223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.3943661971830985E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.12373403786878027</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12861072902338377</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.0148883374689825E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.9271758436944941E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.0514766540174892E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.10993274702534919</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.10746904810229349</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.7801171576534507E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.10253034956852421</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.11522553961483779</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.5206806901441742E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.9589791975558247E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.15709173842947582</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.1507602124931306</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2478-4672-B213-1EA7FF9603CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AH$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AN % AS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mm/yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>43887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43897</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43900</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43902</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43916</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43917</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43920</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AH$2:$AH$35</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.76882430647291944</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.75756533700137552</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.80868486352357316</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.80402605091770274</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.78996865203761757</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.75814795654423173</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.76263446316216765</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.76636386790050093</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.74681878016673975</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.73213131704795142</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.78321909714015603</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.7511344745473334</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.67508159333097406</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.69139647066007204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2478-4672-B213-1EA7FF9603CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="411205248"/>
+        <c:axId val="405728960"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="411205248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="dd/mm/yy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405728960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="405728960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411205248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9907,6 +10974,46 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -13545,6 +14652,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -13591,15 +15203,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13833,95 +15445,141 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AB1C0B-F9B8-4988-9F07-AC2803F63C42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6B74BB9A-8C89-49AE-8A26-574C17DED61A}" name="Data" displayName="Data" ref="A1:AM35" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
-  <autoFilter ref="A1:AM35" xr:uid="{4B85C8C0-D087-4D48-9E65-AF70C439B36D}"/>
-  <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{537F76B1-0773-408D-AD11-67AD04BFF52D}" name="Date" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{0008A3F2-641C-4618-8519-1BB2BB8CD8F1}" name="AS (Acc. Suspects)" dataDxfId="59"/>
-    <tableColumn id="33" xr3:uid="{B1F41BDB-6F83-45BD-886D-945164699B24}" name="AC (Acc. Confirmed)" dataDxfId="58"/>
-    <tableColumn id="35" xr3:uid="{D8AF82E6-615D-4268-9F5D-45734AB5BB49}" name="AR (Acc. Recovered)" dataDxfId="57"/>
-    <tableColumn id="34" xr3:uid="{27A2DFCD-0B9B-4F48-B9EF-2777BE72D531}" name="AD (Acc. Deaths)" dataDxfId="56"/>
-    <tableColumn id="39" xr3:uid="{A6FE9DB6-7EF5-4D96-B970-1E4084DE08C6}" name="AN (Acc. Negatives)" dataDxfId="55"/>
-    <tableColumn id="38" xr3:uid="{F3572767-B889-4E30-A84E-C02E3F871279}" name="AH (Acc. Hospital)" dataDxfId="54"/>
-    <tableColumn id="40" xr3:uid="{904CA045-71CF-4120-9C54-29CFD3B51156}" name="AI (Acc. ICU)" dataDxfId="53"/>
-    <tableColumn id="37" xr3:uid="{1713B47D-516C-43E5-BB78-70FCE1C56DFC}" name="AL (Acc. Pending Lab)" dataDxfId="52"/>
-    <tableColumn id="36" xr3:uid="{14A03D4F-82FF-430E-B0F4-6CB3B0E8AFA8}" name="AV (Acc. Surveillance)" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{B05831DB-9EFA-484C-8251-3E968EF874D8}" name="DNS (Daily New Suspects)" dataDxfId="50"/>
-    <tableColumn id="44" xr3:uid="{77353AAF-2FDA-4BBD-8786-4C210674B1BF}" name="DNC (Daily New Confirmed)" dataDxfId="49"/>
-    <tableColumn id="45" xr3:uid="{C6181719-CC5E-4E1A-AC6B-2A5D74E2B3E8}" name="DNR (Daily New Recovered)" dataDxfId="48"/>
-    <tableColumn id="46" xr3:uid="{51A594EE-5359-44DA-B689-56648C363749}" name="DND (Daily New Deaths)" dataDxfId="47"/>
-    <tableColumn id="47" xr3:uid="{B7648E74-EBC4-484E-88B3-0045CEEB410F}" name="DNN (Daily New Negatives)" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6B74BB9A-8C89-49AE-8A26-574C17DED61A}" name="Data" displayName="Data" ref="A1:AN35" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+  <autoFilter ref="A1:AN35" xr:uid="{4B85C8C0-D087-4D48-9E65-AF70C439B36D}"/>
+  <tableColumns count="40">
+    <tableColumn id="1" xr3:uid="{537F76B1-0773-408D-AD11-67AD04BFF52D}" name="Date" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{0008A3F2-641C-4618-8519-1BB2BB8CD8F1}" name="AS (Acc. Suspects)" dataDxfId="60"/>
+    <tableColumn id="33" xr3:uid="{B1F41BDB-6F83-45BD-886D-945164699B24}" name="AC (Acc. Confirmed)" dataDxfId="59"/>
+    <tableColumn id="35" xr3:uid="{D8AF82E6-615D-4268-9F5D-45734AB5BB49}" name="AR (Acc. Recovered)" dataDxfId="58"/>
+    <tableColumn id="34" xr3:uid="{27A2DFCD-0B9B-4F48-B9EF-2777BE72D531}" name="AD (Acc. Deaths)" dataDxfId="57"/>
+    <tableColumn id="39" xr3:uid="{A6FE9DB6-7EF5-4D96-B970-1E4084DE08C6}" name="AN (Acc. Negatives)" dataDxfId="56"/>
+    <tableColumn id="38" xr3:uid="{F3572767-B889-4E30-A84E-C02E3F871279}" name="AH (Acc. Hospital)" dataDxfId="55"/>
+    <tableColumn id="40" xr3:uid="{904CA045-71CF-4120-9C54-29CFD3B51156}" name="AI (Acc. ICU)" dataDxfId="54"/>
+    <tableColumn id="37" xr3:uid="{1713B47D-516C-43E5-BB78-70FCE1C56DFC}" name="AL (Acc. Pending Lab)" dataDxfId="53"/>
+    <tableColumn id="36" xr3:uid="{14A03D4F-82FF-430E-B0F4-6CB3B0E8AFA8}" name="AV (Acc. Surveillance)" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{B05831DB-9EFA-484C-8251-3E968EF874D8}" name="DNS (Daily New Suspects)" dataDxfId="51"/>
+    <tableColumn id="44" xr3:uid="{77353AAF-2FDA-4BBD-8786-4C210674B1BF}" name="DNC (Daily New Confirmed)" dataDxfId="50"/>
+    <tableColumn id="45" xr3:uid="{C6181719-CC5E-4E1A-AC6B-2A5D74E2B3E8}" name="DNR (Daily New Recovered)" dataDxfId="49"/>
+    <tableColumn id="46" xr3:uid="{51A594EE-5359-44DA-B689-56648C363749}" name="DND (Daily New Deaths)" dataDxfId="48"/>
+    <tableColumn id="47" xr3:uid="{B7648E74-EBC4-484E-88B3-0045CEEB410F}" name="DNN (Daily New Negatives)" dataDxfId="47">
       <calculatedColumnFormula>Data[[#This Row],[AN (Acc. Negatives)]]-F1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{737786A2-9F98-4CD5-AECE-E2E2D3BADFF1}" name="DNH (Daily New Hospital)" dataDxfId="45">
+    <tableColumn id="42" xr3:uid="{737786A2-9F98-4CD5-AECE-E2E2D3BADFF1}" name="DNH (Daily New Hospital)" dataDxfId="46">
       <calculatedColumnFormula>Data[[#This Row],[AH (Acc. Hospital)]]-G1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{BFCA8C58-56C5-48D8-B0D3-B4B44031A59A}" name="DNI (Daily New ICU)" dataDxfId="44">
+    <tableColumn id="43" xr3:uid="{BFCA8C58-56C5-48D8-B0D3-B4B44031A59A}" name="DNI (Daily New ICU)" dataDxfId="45">
       <calculatedColumnFormula>Data[[#This Row],[AI (Acc. ICU)]]-H1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{6CACEBF4-593A-46BC-A478-6480A9259D84}" name="DNL (Daily New Pending Lab)" dataDxfId="43">
+    <tableColumn id="48" xr3:uid="{6CACEBF4-593A-46BC-A478-6480A9259D84}" name="DNL (Daily New Pending Lab)" dataDxfId="44">
       <calculatedColumnFormula>Data[[#This Row],[AL (Acc. Pending Lab)]]-I1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{ABA14777-C6C0-4F6C-BC57-D83D38487AE9}" name="DNV (Daily New Surveillance)" dataDxfId="42">
+    <tableColumn id="41" xr3:uid="{ABA14777-C6C0-4F6C-BC57-D83D38487AE9}" name="DNV (Daily New Surveillance)" dataDxfId="43">
       <calculatedColumnFormula>Data[[#This Row],[AV (Acc. Surveillance)]]-J1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{DE0E97D8-28EF-47F0-8805-8CD1C1585AC7}" name="Active Cases" dataDxfId="41">
+    <tableColumn id="49" xr3:uid="{DE0E97D8-28EF-47F0-8805-8CD1C1585AC7}" name="Active Cases" dataDxfId="42">
       <calculatedColumnFormula>(Data[[#This Row],[AC (Acc. Confirmed)]])-(Data[[#This Row],[AR (Acc. Recovered)]]+Data[[#This Row],[AD (Acc. Deaths)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{9C475E65-DFCB-436A-AD23-8D3E4AD41443}" name="DNS / Prev AS" dataDxfId="40">
+    <tableColumn id="53" xr3:uid="{9C475E65-DFCB-436A-AD23-8D3E4AD41443}" name="DNS / Prev AS" dataDxfId="41">
       <calculatedColumnFormula>Data[[#This Row],[DNS (Daily New Suspects)]]/B1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" xr3:uid="{F83577D1-CD7F-4B76-8269-2AAC4EE28699}" name="DNC / Prev AC" dataDxfId="39">
+    <tableColumn id="50" xr3:uid="{F83577D1-CD7F-4B76-8269-2AAC4EE28699}" name="DNC / Prev AC" dataDxfId="40">
       <calculatedColumnFormula>Data[[#This Row],[DNC (Daily New Confirmed)]]/C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="56" xr3:uid="{9C72D354-7A51-4C64-8E4D-6DD3F10A82AE}" name="DNR / Prev AR" dataDxfId="38" dataCellStyle="Percent">
+    <tableColumn id="56" xr3:uid="{9C72D354-7A51-4C64-8E4D-6DD3F10A82AE}" name="DNR / Prev AR" dataDxfId="39" dataCellStyle="Percent">
       <calculatedColumnFormula>Data[[#This Row],[DNR (Daily New Recovered)]]/D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="57" xr3:uid="{C219B621-113A-4218-B8D9-7CBAFE2631DD}" name="DND / Prev AD" dataDxfId="37" dataCellStyle="Percent">
+    <tableColumn id="57" xr3:uid="{C219B621-113A-4218-B8D9-7CBAFE2631DD}" name="DND / Prev AD" dataDxfId="38" dataCellStyle="Percent">
       <calculatedColumnFormula>Data[[#This Row],[DND (Daily New Deaths)]]/E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="58" xr3:uid="{00EF6CA8-850A-4528-96CE-B66FA03F79D4}" name="Dif DNS vs Prev DNS" dataDxfId="36" dataCellStyle="Comma">
+    <tableColumn id="58" xr3:uid="{00EF6CA8-850A-4528-96CE-B66FA03F79D4}" name="Dif DNS vs Prev DNS" dataDxfId="37" dataCellStyle="Comma">
       <calculatedColumnFormula>Data[[#This Row],[DNS (Daily New Suspects)]]-K1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{73F5E75A-2729-485C-9F78-BC5C00CF8374}" name="Dif DNC vs Prev DNC" dataDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="54" xr3:uid="{73F5E75A-2729-485C-9F78-BC5C00CF8374}" name="Dif DNC vs Prev DNC" dataDxfId="36" dataCellStyle="Percent">
       <calculatedColumnFormula>Data[[#This Row],[DNC (Daily New Confirmed)]]-L1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="60" xr3:uid="{A41CC914-5342-480D-A1C2-03187BEF256A}" name="AC % AS" dataDxfId="34" dataCellStyle="Percent">
+    <tableColumn id="60" xr3:uid="{A41CC914-5342-480D-A1C2-03187BEF256A}" name="AC % AS" dataDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>Data[[#This Row],[AC (Acc. Confirmed)]]/Data[[#This Row],[AS (Acc. Suspects)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="61" xr3:uid="{33847944-B458-4C0F-84FD-F9F641CE2A31}" name="AR % AC" dataDxfId="33" dataCellStyle="Percent">
+    <tableColumn id="61" xr3:uid="{33847944-B458-4C0F-84FD-F9F641CE2A31}" name="AR % AC" dataDxfId="34" dataCellStyle="Percent">
       <calculatedColumnFormula>Data[[#This Row],[AR (Acc. Recovered)]]/Data[[#This Row],[AS (Acc. Suspects)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{5EE34295-D892-40E8-B845-3100DD1F58B6}" name="AD % AC" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="55" xr3:uid="{5EE34295-D892-40E8-B845-3100DD1F58B6}" name="AD % AC" dataDxfId="33" dataCellStyle="Percent">
       <calculatedColumnFormula>Data[[#This Row],[AD (Acc. Deaths)]]/Data[[#This Row],[AS (Acc. Suspects)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{E97E275F-04DE-439A-8ACF-32433CE3A541}" name="AC % AN" dataDxfId="31">
+    <tableColumn id="51" xr3:uid="{E97E275F-04DE-439A-8ACF-32433CE3A541}" name="AC % AN" dataDxfId="32">
       <calculatedColumnFormula>Data[[#This Row],[AC (Acc. Confirmed)]]/Data[[#This Row],[AN (Acc. Negatives)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{C4A93212-B0D1-4EDC-BBB7-434A9E69C6D7}" name="AH % AC" dataDxfId="30">
+    <tableColumn id="66" xr3:uid="{C4A93212-B0D1-4EDC-BBB7-434A9E69C6D7}" name="AH % AC" dataDxfId="31">
       <calculatedColumnFormula>Data[[#This Row],[AH (Acc. Hospital)]]/Data[[#This Row],[AC (Acc. Confirmed)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{FF08FDE4-B4F4-4855-A23B-2D2C917DBED6}" name="AI % AH" dataDxfId="29">
+    <tableColumn id="67" xr3:uid="{FF08FDE4-B4F4-4855-A23B-2D2C917DBED6}" name="AI % AH" dataDxfId="30">
       <calculatedColumnFormula>Data[[#This Row],[AI (Acc. ICU)]]/Data[[#This Row],[AH (Acc. Hospital)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{05B1C735-9629-4AE5-9401-D9B2E627C503}" name="AL % AS" dataDxfId="28">
+    <tableColumn id="65" xr3:uid="{05B1C735-9629-4AE5-9401-D9B2E627C503}" name="AL % AS" dataDxfId="29">
       <calculatedColumnFormula>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{91D01986-5984-4F08-AC6D-83F70AB781EE}" name="DNC % DNS" dataDxfId="27">
+    <tableColumn id="6" xr3:uid="{4BDCE953-A35F-4789-86A5-F98C4AA344AF}" name="AN % AS" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{91D01986-5984-4F08-AC6D-83F70AB781EE}" name="DNC % DNS" dataDxfId="28">
       <calculatedColumnFormula>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{A40F9A6C-FD69-41C8-BF89-8A30C5CA176D}" name="DNC % DNN" dataDxfId="26">
+    <tableColumn id="64" xr3:uid="{A40F9A6C-FD69-41C8-BF89-8A30C5CA176D}" name="DNC % DNN" dataDxfId="27">
       <calculatedColumnFormula>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{0951DA88-EDD7-4580-89E9-23D53B670CAC}" name="Report ID" dataDxfId="25"/>
-    <tableColumn id="21" xr3:uid="{F7DAFDBF-582E-46C5-A32A-B945C74E2942}" name="Week" dataDxfId="24">
+    <tableColumn id="25" xr3:uid="{0951DA88-EDD7-4580-89E9-23D53B670CAC}" name="Report ID" dataDxfId="26"/>
+    <tableColumn id="21" xr3:uid="{F7DAFDBF-582E-46C5-A32A-B945C74E2942}" name="Week" dataDxfId="25">
       <calculatedColumnFormula>WEEKNUM(Data[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{75E95CD2-5E14-44E8-AC6C-3D702007373D}" name="Month" dataDxfId="23">
+    <tableColumn id="22" xr3:uid="{75E95CD2-5E14-44E8-AC6C-3D702007373D}" name="Month" dataDxfId="24">
       <calculatedColumnFormula>MONTH(Data[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{17EBFFFD-C3E6-4217-8A7D-0CC76F549881}" name="Weekday" dataDxfId="22">
+    <tableColumn id="23" xr3:uid="{17EBFFFD-C3E6-4217-8A7D-0CC76F549881}" name="Weekday" dataDxfId="23">
       <calculatedColumnFormula>WEEKDAY(Data[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13930,13 +15588,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BE8B474E-7313-4CDA-898A-F42D1BB90707}" name="Table4" displayName="Table4" ref="A1:D66" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BE8B474E-7313-4CDA-898A-F42D1BB90707}" name="Table4" displayName="Table4" ref="A1:D66" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20" dataCellStyle="Comma">
   <autoFilter ref="A1:D66" xr:uid="{F215F903-A661-4A02-88A8-B5EF1B6BD985}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FE63B76F-DE7C-4023-925A-5B0E6DE82229}" name="Timeline" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{76C9CB77-B863-4452-ACBD-78363520B942}" name="Actuals" dataDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{3D0DE8D3-36AD-43B3-8007-CC9DC167A0C2}" name="FCT0328" dataDxfId="16" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{1503E8D9-37AB-49BD-BEFE-2B53D0459014}" name="FCT0327" dataDxfId="15" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{FE63B76F-DE7C-4023-925A-5B0E6DE82229}" name="Timeline" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{76C9CB77-B863-4452-ACBD-78363520B942}" name="Actuals" dataDxfId="18" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{3D0DE8D3-36AD-43B3-8007-CC9DC167A0C2}" name="FCT0328" dataDxfId="17" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{1503E8D9-37AB-49BD-BEFE-2B53D0459014}" name="FCT0327" dataDxfId="16" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13946,15 +15604,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D2B141E4-3E13-47A2-8341-A7D5FD70E2CF}" name="Table10" displayName="Table10" ref="A1:E66" totalsRowShown="0">
   <autoFilter ref="A1:E66" xr:uid="{D9EA3EA6-45E8-42E0-9715-75DEE5808C87}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{32815590-5F9F-4781-86BA-E237D749AADB}" name="Timeline" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{32815590-5F9F-4781-86BA-E237D749AADB}" name="Timeline" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{4FC79A25-59CB-44F5-804A-032F4DDBD6D6}" name="Values"/>
-    <tableColumn id="3" xr3:uid="{34C1C7E1-EF41-4104-8FB5-67AAA80840BF}" name="Forecast" dataDxfId="13">
+    <tableColumn id="3" xr3:uid="{34C1C7E1-EF41-4104-8FB5-67AAA80840BF}" name="Forecast" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.FORECAST.ETS(A2,$B$2:$B$33,$A$2:$A$33,1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{425B71B7-6019-4334-BE7B-DFDC22BA49E9}" name="Lower Confidence Bound" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{425B71B7-6019-4334-BE7B-DFDC22BA49E9}" name="Lower Confidence Bound" dataDxfId="13">
       <calculatedColumnFormula>C2-_xlfn.FORECAST.ETS.CONFINT(A2,$B$2:$B$33,$A$2:$A$33,0.95,1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5981AE1E-B24D-4B97-A76E-B02532A2B6CF}" name="Upper Confidence Bound" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{5981AE1E-B24D-4B97-A76E-B02532A2B6CF}" name="Upper Confidence Bound" dataDxfId="12">
       <calculatedColumnFormula>C2+_xlfn.FORECAST.ETS.CONFINT(A2,$B$2:$B$33,$A$2:$A$33,0.95,1,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13967,20 +15625,20 @@
   <autoFilter ref="G1:H8" xr:uid="{1F91246C-2F26-43E7-AD66-C817792AE31B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{09F47A8E-4996-4E18-8F23-ED854F034072}" name="Statistic"/>
-    <tableColumn id="2" xr3:uid="{7AC38D9D-B81C-4406-B973-92EAE7C710C8}" name="Value" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{7AC38D9D-B81C-4406-B973-92EAE7C710C8}" name="Value" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{34145EB7-FBE8-4E3C-BA3F-75F6EB17DE4B}" name="Table14" displayName="Table14" ref="A1:D66" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{34145EB7-FBE8-4E3C-BA3F-75F6EB17DE4B}" name="Table14" displayName="Table14" ref="A1:D66" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:D66" xr:uid="{55C7C5FF-BF58-4905-B69E-C7F94EE3A837}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{517BE8E7-591D-46F8-B234-3EF76B78A8F9}" name="Timeline" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1AE710DC-7759-41C5-A500-5EF63D1BA08E}" name="Actuals" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{378540BE-10CE-4A1C-9BD2-ECA3074D046B}" name="FCT0328" dataDxfId="6" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{E9BC202A-278C-4191-A924-F7FD31E1146E}" name="FCT0327" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{517BE8E7-591D-46F8-B234-3EF76B78A8F9}" name="Timeline" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1AE710DC-7759-41C5-A500-5EF63D1BA08E}" name="Actuals" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{378540BE-10CE-4A1C-9BD2-ECA3074D046B}" name="FCT0328" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{E9BC202A-278C-4191-A924-F7FD31E1146E}" name="FCT0327" dataDxfId="6" dataCellStyle="Comma">
       <calculatedColumnFormula>_xlfn.FORECAST.ETS(A2,$B$2:$B$32,$A$2:$A$32,1,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13992,15 +15650,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{7F4E325E-9B44-4284-9987-040E42758C27}" name="Table12" displayName="Table12" ref="A1:E66" totalsRowShown="0">
   <autoFilter ref="A1:E66" xr:uid="{D0C0E5A0-150E-4BC3-9A54-36FD983DE47B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C9B50D03-8250-4543-95CD-EED0624019CD}" name="Timeline" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C9B50D03-8250-4543-95CD-EED0624019CD}" name="Timeline" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{B5B0FC7D-9517-44D6-9EFA-E23CB1F07F14}" name="Values"/>
-    <tableColumn id="3" xr3:uid="{690E0446-C719-4EFF-8C54-EDED600BC934}" name="Forecast" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{690E0446-C719-4EFF-8C54-EDED600BC934}" name="Forecast" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.FORECAST.ETS(A2,$B$2:$B$33,$A$2:$A$33,1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{302C5B06-359C-48AD-96B4-88516234CA9D}" name="Lower Confidence Bound" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{302C5B06-359C-48AD-96B4-88516234CA9D}" name="Lower Confidence Bound" dataDxfId="3">
       <calculatedColumnFormula>C2-_xlfn.FORECAST.ETS.CONFINT(A2,$B$2:$B$33,$A$2:$A$33,0.95,1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B1AF5A24-6EE5-4688-B674-AFA90988AD46}" name="Upper Confidence Bound" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{B1AF5A24-6EE5-4688-B674-AFA90988AD46}" name="Upper Confidence Bound" dataDxfId="2">
       <calculatedColumnFormula>C2+_xlfn.FORECAST.ETS.CONFINT(A2,$B$2:$B$33,$A$2:$A$33,0.95,1,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14013,7 +15671,7 @@
   <autoFilter ref="G1:H8" xr:uid="{E86A0924-9A27-4453-9FD7-C3E173E2122A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{87A794F4-5475-4B4D-932F-D4BAE1311704}" name="Statistic"/>
-    <tableColumn id="2" xr3:uid="{0F5AF389-9B84-4B90-9338-C87DA3DC7DE5}" name="Value" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0F5AF389-9B84-4B90-9338-C87DA3DC7DE5}" name="Value" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14316,11 +15974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A4BEF7-1EBF-4C6F-A5A0-018842EA1507}">
-  <dimension ref="A1:AM35"/>
+  <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="1" sqref="U23:X33 A23:A33"/>
+      <selection pane="bottomLeft" activeCell="AH1" activeCellId="3" sqref="A1:A1048576 AA1:AA1048576 AG1:AG1048576 AH1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -14331,13 +15989,13 @@
     <col min="20" max="24" width="5.7109375" style="38" customWidth="1"/>
     <col min="25" max="25" width="5.7109375" style="39" customWidth="1"/>
     <col min="26" max="28" width="5.7109375" style="40" customWidth="1"/>
-    <col min="29" max="33" width="5.7109375" style="38" customWidth="1"/>
-    <col min="34" max="35" width="5.7109375" style="10" customWidth="1"/>
-    <col min="36" max="39" width="5.7109375" style="41" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="10"/>
+    <col min="29" max="34" width="5.7109375" style="38" customWidth="1"/>
+    <col min="35" max="36" width="5.7109375" style="10" customWidth="1"/>
+    <col min="37" max="40" width="5.7109375" style="41" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14437,26 +16095,29 @@
       <c r="AG1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AM1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AN1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>43887</v>
       </c>
@@ -14523,26 +16184,30 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH2" s="20">
+      <c r="AH2" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22">
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>9</v>
       </c>
-      <c r="AL2" s="22">
+      <c r="AM2" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
-      <c r="AM2" s="23">
+      <c r="AN2" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>43888</v>
       </c>
@@ -14633,26 +16298,30 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH3" s="20">
+      <c r="AH3" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="22">
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>9</v>
       </c>
-      <c r="AL3" s="22">
+      <c r="AM3" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
-      <c r="AM3" s="23">
+      <c r="AN3" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>43889</v>
       </c>
@@ -14743,26 +16412,30 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="20">
+      <c r="AH4" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AI4" s="21"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22">
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>9</v>
       </c>
-      <c r="AL4" s="22">
+      <c r="AM4" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
-      <c r="AM4" s="23">
+      <c r="AN4" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>43890</v>
       </c>
@@ -14853,26 +16526,30 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH5" s="20">
+      <c r="AH5" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="22"/>
-      <c r="AK5" s="22">
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="22"/>
+      <c r="AL5" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>9</v>
       </c>
-      <c r="AL5" s="22">
+      <c r="AM5" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
-      <c r="AM5" s="23">
+      <c r="AN5" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>43891</v>
       </c>
@@ -14965,26 +16642,30 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH6" s="20">
+      <c r="AH6" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AI6" s="21"/>
-      <c r="AJ6" s="22"/>
-      <c r="AK6" s="22">
+      <c r="AJ6" s="21"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL6" s="22">
+      <c r="AM6" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM6" s="23">
+      <c r="AN6" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>43892</v>
       </c>
@@ -15078,23 +16759,27 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="22"/>
-      <c r="AK7" s="22">
+      <c r="AH7" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="21"/>
+      <c r="AK7" s="22"/>
+      <c r="AL7" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL7" s="22">
+      <c r="AM7" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM7" s="23">
+      <c r="AN7" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>43893</v>
       </c>
@@ -15193,28 +16878,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH8" s="20">
+      <c r="AH8" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.125</v>
       </c>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="22">
+      <c r="AJ8" s="21"/>
+      <c r="AK8" s="22">
         <v>1</v>
       </c>
-      <c r="AK8" s="22">
+      <c r="AL8" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL8" s="22">
+      <c r="AM8" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM8" s="23">
+      <c r="AN8" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>43894</v>
       </c>
@@ -15313,28 +17002,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH9" s="20">
+      <c r="AH9" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.125</v>
       </c>
-      <c r="AI9" s="21"/>
-      <c r="AJ9" s="22">
+      <c r="AJ9" s="21"/>
+      <c r="AK9" s="22">
         <v>2</v>
       </c>
-      <c r="AK9" s="22">
+      <c r="AL9" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL9" s="22">
+      <c r="AM9" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM9" s="23">
+      <c r="AN9" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>43895</v>
       </c>
@@ -15438,28 +17131,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0</v>
       </c>
-      <c r="AH10" s="20">
+      <c r="AH10" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.1</v>
       </c>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="22">
+      <c r="AJ10" s="21"/>
+      <c r="AK10" s="22">
         <v>3</v>
       </c>
-      <c r="AK10" s="22">
+      <c r="AL10" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL10" s="22">
+      <c r="AM10" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM10" s="23">
+      <c r="AN10" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>43896</v>
       </c>
@@ -15565,28 +17262,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.16574585635359115</v>
       </c>
-      <c r="AH11" s="20">
+      <c r="AH11" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.11764705882352941</v>
       </c>
-      <c r="AI11" s="21"/>
-      <c r="AJ11" s="22">
+      <c r="AJ11" s="21"/>
+      <c r="AK11" s="22">
         <v>4</v>
       </c>
-      <c r="AK11" s="22">
+      <c r="AL11" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL11" s="22">
+      <c r="AM11" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM11" s="23">
+      <c r="AN11" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>43897</v>
       </c>
@@ -15692,28 +17393,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.20982142857142858</v>
       </c>
-      <c r="AH12" s="20">
+      <c r="AH12" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.18604651162790697</v>
       </c>
-      <c r="AI12" s="21"/>
-      <c r="AJ12" s="22">
+      <c r="AJ12" s="21"/>
+      <c r="AK12" s="22">
         <v>5</v>
       </c>
-      <c r="AK12" s="22">
+      <c r="AL12" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>10</v>
       </c>
-      <c r="AL12" s="22">
+      <c r="AM12" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM12" s="23">
+      <c r="AN12" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>43898</v>
       </c>
@@ -15819,28 +17524,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.199288256227758</v>
       </c>
-      <c r="AH13" s="20">
+      <c r="AH13" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.15789473684210525</v>
       </c>
-      <c r="AI13" s="21"/>
-      <c r="AJ13" s="22">
+      <c r="AJ13" s="21"/>
+      <c r="AK13" s="22">
         <v>6</v>
       </c>
-      <c r="AK13" s="22">
+      <c r="AL13" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL13" s="22">
+      <c r="AM13" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM13" s="23">
+      <c r="AN13" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>43899</v>
       </c>
@@ -15946,28 +17655,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.19764011799410031</v>
       </c>
-      <c r="AH14" s="20">
+      <c r="AH14" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.15517241379310345</v>
       </c>
-      <c r="AI14" s="21"/>
-      <c r="AJ14" s="22">
+      <c r="AJ14" s="21"/>
+      <c r="AK14" s="22">
         <v>7</v>
       </c>
-      <c r="AK14" s="22">
+      <c r="AL14" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL14" s="22">
+      <c r="AM14" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM14" s="23">
+      <c r="AN14" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>43900</v>
       </c>
@@ -16073,28 +17786,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.22133333333333333</v>
       </c>
-      <c r="AH15" s="20">
+      <c r="AH15" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AI15" s="21"/>
-      <c r="AJ15" s="22">
+      <c r="AJ15" s="21"/>
+      <c r="AK15" s="22">
         <v>8</v>
       </c>
-      <c r="AK15" s="22">
+      <c r="AL15" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL15" s="22">
+      <c r="AM15" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM15" s="23">
+      <c r="AN15" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>43901</v>
       </c>
@@ -16200,28 +17917,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.17622080679405519</v>
       </c>
-      <c r="AH16" s="20">
+      <c r="AH16" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.1875</v>
       </c>
-      <c r="AI16" s="21"/>
-      <c r="AJ16" s="22">
+      <c r="AJ16" s="21"/>
+      <c r="AK16" s="22">
         <v>9</v>
       </c>
-      <c r="AK16" s="22">
+      <c r="AL16" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL16" s="22">
+      <c r="AM16" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM16" s="23">
+      <c r="AN16" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>43902</v>
       </c>
@@ -16327,28 +18048,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.2087912087912088</v>
       </c>
-      <c r="AH17" s="20">
+      <c r="AH17" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.1144578313253012</v>
       </c>
-      <c r="AI17" s="21"/>
-      <c r="AJ17" s="22">
+      <c r="AJ17" s="21"/>
+      <c r="AK17" s="22">
         <v>10</v>
       </c>
-      <c r="AK17" s="22">
+      <c r="AL17" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL17" s="22">
+      <c r="AM17" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM17" s="23">
+      <c r="AN17" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>43903</v>
       </c>
@@ -16454,28 +18179,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.13149847094801223</v>
       </c>
-      <c r="AH18" s="20">
+      <c r="AH18" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>5.0670640834575259E-2</v>
       </c>
-      <c r="AI18" s="21"/>
-      <c r="AJ18" s="22">
+      <c r="AJ18" s="21"/>
+      <c r="AK18" s="22">
         <v>11</v>
       </c>
-      <c r="AK18" s="22">
+      <c r="AL18" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL18" s="22">
+      <c r="AM18" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM18" s="23">
+      <c r="AN18" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>43904</v>
       </c>
@@ -16583,28 +18312,32 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>7.3943661971830985E-2</v>
       </c>
-      <c r="AH19" s="20">
+      <c r="AH19" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI19" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.14393939393939395</v>
       </c>
-      <c r="AI19" s="24"/>
-      <c r="AJ19" s="22">
+      <c r="AJ19" s="24"/>
+      <c r="AK19" s="22">
         <v>12</v>
       </c>
-      <c r="AK19" s="22">
+      <c r="AL19" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>11</v>
       </c>
-      <c r="AL19" s="22">
+      <c r="AM19" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM19" s="23">
+      <c r="AN19" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>43905</v>
       </c>
@@ -16720,31 +18453,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.12373403786878027</v>
       </c>
-      <c r="AH20" s="20">
+      <c r="AH20" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.76882430647291944</v>
+      </c>
+      <c r="AI20" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.13403880070546736</v>
       </c>
-      <c r="AI20" s="25">
+      <c r="AJ20" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>4.3528064146620846E-2</v>
       </c>
-      <c r="AJ20" s="22">
+      <c r="AK20" s="22">
         <v>13</v>
       </c>
-      <c r="AK20" s="22">
+      <c r="AL20" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL20" s="22">
+      <c r="AM20" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM20" s="23">
+      <c r="AN20" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>43906</v>
       </c>
@@ -16860,31 +18597,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.12861072902338377</v>
       </c>
-      <c r="AH21" s="20">
+      <c r="AH21" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.75756533700137552</v>
+      </c>
+      <c r="AI21" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.13500784929356358</v>
       </c>
-      <c r="AI21" s="25">
+      <c r="AJ21" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.18818380743982493</v>
       </c>
-      <c r="AJ21" s="22">
+      <c r="AK21" s="22">
         <v>14</v>
       </c>
-      <c r="AK21" s="22">
+      <c r="AL21" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL21" s="22">
+      <c r="AM21" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM21" s="23">
+      <c r="AN21" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>43907</v>
       </c>
@@ -17000,31 +18741,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>8.0148883374689825E-2</v>
       </c>
-      <c r="AH22" s="20">
+      <c r="AH22" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.80868486352357316</v>
+      </c>
+      <c r="AI22" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.10427807486631016</v>
       </c>
-      <c r="AI22" s="25">
+      <c r="AJ22" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.11079545454545454</v>
       </c>
-      <c r="AJ22" s="22">
+      <c r="AK22" s="22">
         <v>15</v>
       </c>
-      <c r="AK22" s="22">
+      <c r="AL22" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL22" s="22">
+      <c r="AM22" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM22" s="23">
+      <c r="AN22" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>43908</v>
       </c>
@@ -17143,31 +18888,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>6.9271758436944941E-2</v>
       </c>
-      <c r="AH23" s="20">
+      <c r="AH23" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.80402605091770274</v>
+      </c>
+      <c r="AI23" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.1870781099324976</v>
       </c>
-      <c r="AI23" s="25">
+      <c r="AJ23" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.23803680981595093</v>
       </c>
-      <c r="AJ23" s="22">
+      <c r="AK23" s="22">
         <v>16</v>
       </c>
-      <c r="AK23" s="22">
+      <c r="AL23" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL23" s="22">
+      <c r="AM23" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM23" s="23">
+      <c r="AN23" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>43909</v>
       </c>
@@ -17286,31 +19035,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>8.0514766540174892E-2</v>
       </c>
-      <c r="AH24" s="20">
+      <c r="AH24" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.78996865203761757</v>
+      </c>
+      <c r="AI24" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.14386317907444668</v>
       </c>
-      <c r="AI24" s="25">
+      <c r="AJ24" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.20028011204481794</v>
       </c>
-      <c r="AJ24" s="22">
+      <c r="AK24" s="22">
         <v>17</v>
       </c>
-      <c r="AK24" s="22">
+      <c r="AL24" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL24" s="22">
+      <c r="AM24" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM24" s="23">
+      <c r="AN24" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>43910</v>
       </c>
@@ -17429,31 +19182,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.10993274702534919</v>
       </c>
-      <c r="AH25" s="20">
+      <c r="AH25" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.75814795654423173</v>
+      </c>
+      <c r="AI25" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.14063435068821065</v>
       </c>
-      <c r="AI25" s="25">
+      <c r="AJ25" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.21880819366852886</v>
       </c>
-      <c r="AJ25" s="22">
+      <c r="AK25" s="22">
         <v>18</v>
       </c>
-      <c r="AK25" s="22">
+      <c r="AL25" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL25" s="22">
+      <c r="AM25" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM25" s="23">
+      <c r="AN25" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>43911</v>
       </c>
@@ -17572,31 +19329,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.10746904810229349</v>
       </c>
-      <c r="AH26" s="20">
+      <c r="AH26" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.76263446316216765</v>
+      </c>
+      <c r="AI26" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.12252591894439209</v>
       </c>
-      <c r="AI26" s="25">
+      <c r="AJ26" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.15728977616454931</v>
       </c>
-      <c r="AJ26" s="22">
+      <c r="AK26" s="22">
         <v>19</v>
       </c>
-      <c r="AK26" s="22">
+      <c r="AL26" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>12</v>
       </c>
-      <c r="AL26" s="22">
+      <c r="AM26" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM26" s="23">
+      <c r="AN26" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>43912</v>
       </c>
@@ -17715,31 +19476,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>9.7801171576534507E-2</v>
       </c>
-      <c r="AH27" s="20">
+      <c r="AH27" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.76636386790050093</v>
+      </c>
+      <c r="AI27" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.16623376623376623</v>
       </c>
-      <c r="AI27" s="25">
+      <c r="AJ27" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.21164021164021163</v>
       </c>
-      <c r="AJ27" s="22">
+      <c r="AK27" s="22">
         <v>20</v>
       </c>
-      <c r="AK27" s="22">
+      <c r="AL27" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL27" s="22">
+      <c r="AM27" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM27" s="23">
+      <c r="AN27" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>43913</v>
       </c>
@@ -17858,31 +19623,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.10253034956852421</v>
       </c>
-      <c r="AH28" s="20">
+      <c r="AH28" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.74681878016673975</v>
+      </c>
+      <c r="AI28" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.24274406332453827</v>
       </c>
-      <c r="AI28" s="25">
+      <c r="AJ28" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.3881856540084388</v>
       </c>
-      <c r="AJ28" s="22">
+      <c r="AK28" s="22">
         <v>21</v>
       </c>
-      <c r="AK28" s="22">
+      <c r="AL28" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL28" s="22">
+      <c r="AM28" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM28" s="23">
+      <c r="AN28" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>43914</v>
       </c>
@@ -18001,31 +19770,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.11522553961483779</v>
       </c>
-      <c r="AH29" s="20">
+      <c r="AH29" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.73213131704795142</v>
+      </c>
+      <c r="AI29" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.16777777777777778</v>
       </c>
-      <c r="AI29" s="25">
+      <c r="AJ29" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.27036705461056398</v>
       </c>
-      <c r="AJ29" s="22">
+      <c r="AK29" s="22">
         <v>22</v>
       </c>
-      <c r="AK29" s="22">
+      <c r="AL29" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL29" s="22">
+      <c r="AM29" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM29" s="23">
+      <c r="AN29" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>43915</v>
       </c>
@@ -18144,31 +19917,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>7.5206806901441742E-2</v>
       </c>
-      <c r="AH30" s="20">
+      <c r="AH30" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.78321909714015603</v>
+      </c>
+      <c r="AI30" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.111424045062489</v>
       </c>
-      <c r="AI30" s="25">
+      <c r="AJ30" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.12080152671755726</v>
       </c>
-      <c r="AJ30" s="22">
+      <c r="AK30" s="22">
         <v>23</v>
       </c>
-      <c r="AK30" s="22">
+      <c r="AL30" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL30" s="22">
+      <c r="AM30" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM30" s="23">
+      <c r="AN30" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>43916</v>
       </c>
@@ -18287,31 +20064,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>8.9589791975558247E-2</v>
       </c>
-      <c r="AH31" s="20">
+      <c r="AH31" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.7511344745473334</v>
+      </c>
+      <c r="AI31" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.49818511796733211</v>
       </c>
-      <c r="AI31" s="25">
+      <c r="AJ31" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>3.6845637583892619</v>
       </c>
-      <c r="AJ31" s="22">
+      <c r="AK31" s="22">
         <v>24</v>
       </c>
-      <c r="AK31" s="22">
+      <c r="AL31" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL31" s="22">
+      <c r="AM31" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM31" s="23">
+      <c r="AN31" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>43917</v>
       </c>
@@ -18430,31 +20211,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.15709173842947582</v>
       </c>
-      <c r="AH32" s="20">
+      <c r="AH32" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.67508159333097406</v>
+      </c>
+      <c r="AI32" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.22810333963453056</v>
       </c>
-      <c r="AI32" s="25">
+      <c r="AJ32" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>1.6088888888888888</v>
       </c>
-      <c r="AJ32" s="22">
+      <c r="AK32" s="22">
         <v>25</v>
       </c>
-      <c r="AK32" s="22">
+      <c r="AL32" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL32" s="22">
+      <c r="AM32" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM32" s="23">
+      <c r="AN32" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>43918</v>
       </c>
@@ -18577,31 +20362,35 @@
         <f>Data[[#This Row],[AL (Acc. Pending Lab)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
         <v>0.1507602124931306</v>
       </c>
-      <c r="AH33" s="20">
+      <c r="AH33" s="16">
+        <f>Data[[#This Row],[AN (Acc. Negatives)]]/Data[[#This Row],[AS (Acc. Suspects)]]</f>
+        <v>0.69139647066007204</v>
+      </c>
+      <c r="AI33" s="20">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNS (Daily New Suspects)]]</f>
         <v>0.12317356274750785</v>
       </c>
-      <c r="AI33" s="25">
+      <c r="AJ33" s="25">
         <f>Data[[#This Row],[DNC (Daily New Confirmed)]]/Data[[#This Row],[DNN (Daily New Negatives)]]</f>
         <v>0.1646586345381526</v>
       </c>
-      <c r="AJ33" s="22">
+      <c r="AK33" s="22">
         <v>26</v>
       </c>
-      <c r="AK33" s="22">
+      <c r="AL33" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>13</v>
       </c>
-      <c r="AL33" s="22">
+      <c r="AM33" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM33" s="23">
+      <c r="AN33" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>43919</v>
       </c>
@@ -18637,23 +20426,24 @@
       <c r="AE34" s="26"/>
       <c r="AF34" s="26"/>
       <c r="AG34" s="26"/>
-      <c r="AH34" s="27"/>
-      <c r="AI34" s="28"/>
-      <c r="AJ34" s="22"/>
-      <c r="AK34" s="22">
+      <c r="AH34" s="26"/>
+      <c r="AI34" s="27"/>
+      <c r="AJ34" s="28"/>
+      <c r="AK34" s="22"/>
+      <c r="AL34" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>14</v>
       </c>
-      <c r="AL34" s="22">
+      <c r="AM34" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM34" s="23">
+      <c r="AN34" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>43920</v>
       </c>
@@ -18689,18 +20479,19 @@
       <c r="AE35" s="32"/>
       <c r="AF35" s="32"/>
       <c r="AG35" s="32"/>
-      <c r="AH35" s="35"/>
-      <c r="AI35" s="28"/>
-      <c r="AJ35" s="22"/>
-      <c r="AK35" s="22">
+      <c r="AH35" s="32"/>
+      <c r="AI35" s="35"/>
+      <c r="AJ35" s="28"/>
+      <c r="AK35" s="22"/>
+      <c r="AL35" s="22">
         <f>WEEKNUM(Data[[#This Row],[Date]])</f>
         <v>14</v>
       </c>
-      <c r="AL35" s="22">
+      <c r="AM35" s="22">
         <f>MONTH(Data[[#This Row],[Date]])</f>
         <v>3</v>
       </c>
-      <c r="AM35" s="23">
+      <c r="AN35" s="23">
         <f>WEEKDAY(Data[[#This Row],[Date]])</f>
         <v>2</v>
       </c>
@@ -18715,12 +20506,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A1FC48-1772-41D0-AA7B-D9F7A743284A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BE9A43-4D21-4AF4-86F1-E52B3AF2C5F6}">
   <dimension ref="A4:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18756,31 +20560,31 @@
         <v>18</v>
       </c>
       <c r="B5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!B4),0)</f>
         <v>70</v>
       </c>
       <c r="C5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!C4),0)</f>
         <v>154</v>
       </c>
       <c r="D5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!D4),0)</f>
         <v>1480</v>
       </c>
       <c r="E5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!E4),0)</f>
         <v>8150</v>
       </c>
       <c r="F5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!F4),0)</f>
         <v>22900</v>
       </c>
       <c r="G5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H5" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18789,31 +20593,31 @@
         <v>21</v>
       </c>
       <c r="B6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!C4),0)</f>
         <v>21</v>
       </c>
       <c r="D6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!D4),0)</f>
         <v>148</v>
       </c>
       <c r="E6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!E4),0)</f>
         <v>1111</v>
       </c>
       <c r="F6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!F4),0)</f>
         <v>3890</v>
       </c>
       <c r="G6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18822,31 +20626,31 @@
         <v>19</v>
       </c>
       <c r="B7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!C4),0)</f>
         <v>0</v>
       </c>
       <c r="D7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!D4),0)</f>
         <v>1</v>
       </c>
       <c r="E7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!E4),0)</f>
         <v>4</v>
       </c>
       <c r="F7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!F4),0)</f>
         <v>38</v>
       </c>
       <c r="G7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H7" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18855,31 +20659,31 @@
         <v>20</v>
       </c>
       <c r="B8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!C4),0)</f>
         <v>0</v>
       </c>
       <c r="D8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!D4),0)</f>
         <v>0</v>
       </c>
       <c r="E8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!E4),0)</f>
         <v>12</v>
       </c>
       <c r="F8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!F4),0)</f>
         <v>88</v>
       </c>
       <c r="G8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H8" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18888,31 +20692,31 @@
         <v>22</v>
       </c>
       <c r="B9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!C4),0)</f>
         <v>0</v>
       </c>
       <c r="D9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!D4),0)</f>
         <v>0</v>
       </c>
       <c r="E9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!E4),0)</f>
         <v>7515</v>
       </c>
       <c r="F9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!F4),0)</f>
         <v>15131</v>
       </c>
       <c r="G9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H9" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18921,31 +20725,31 @@
         <v>23</v>
       </c>
       <c r="B10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!C4),0)</f>
         <v>21</v>
       </c>
       <c r="D10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!D4),0)</f>
         <v>93</v>
       </c>
       <c r="E10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!E4),0)</f>
         <v>42</v>
       </c>
       <c r="F10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!F4),0)</f>
         <v>262</v>
       </c>
       <c r="G10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H10" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18954,31 +20758,31 @@
         <v>24</v>
       </c>
       <c r="B11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!C4),0)</f>
         <v>0</v>
       </c>
       <c r="D11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!D4),0)</f>
         <v>10</v>
       </c>
       <c r="E11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!E4),0)</f>
         <v>25</v>
       </c>
       <c r="F11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!F4),0)</f>
         <v>54</v>
       </c>
       <c r="G11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H11" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -18987,31 +20791,31 @@
         <v>25</v>
       </c>
       <c r="B12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!C4),0)</f>
         <v>47</v>
       </c>
       <c r="D12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!D4),0)</f>
         <v>79</v>
       </c>
       <c r="E12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!E4),0)</f>
         <v>933</v>
       </c>
       <c r="F12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!F4),0)</f>
         <v>3879</v>
       </c>
       <c r="G12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H12" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19020,31 +20824,31 @@
         <v>26</v>
       </c>
       <c r="B13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!B4),0)</f>
         <v>0</v>
       </c>
       <c r="C13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!C4),0)</f>
         <v>412</v>
       </c>
       <c r="D13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!D4),0)</f>
         <v>4599</v>
       </c>
       <c r="E13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!E4),0)</f>
         <v>8144</v>
       </c>
       <c r="F13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!F4),0)</f>
         <v>6772</v>
       </c>
       <c r="G13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!G4),0)</f>
         <v>0</v>
       </c>
       <c r="H13" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AK:$AK,Week!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AL:$AL,Week!H4),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -19471,7 +21275,7 @@
   <dimension ref="A4:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19531,31 +21335,31 @@
         <v>18</v>
       </c>
       <c r="B6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>2590</v>
       </c>
       <c r="C6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>2974</v>
       </c>
       <c r="D6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>6855</v>
       </c>
       <c r="E6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>2318</v>
       </c>
       <c r="F6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>5558</v>
       </c>
       <c r="G6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>9895</v>
       </c>
       <c r="H6" s="59">
-        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$K:$K,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>2564</v>
       </c>
     </row>
@@ -19564,31 +21368,31 @@
         <v>21</v>
       </c>
       <c r="B7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>557</v>
       </c>
       <c r="C7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>423</v>
       </c>
       <c r="D7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>847</v>
       </c>
       <c r="E7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>714</v>
       </c>
       <c r="F7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>997</v>
       </c>
       <c r="G7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>1227</v>
       </c>
       <c r="H7" s="59">
-        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$L:$L,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>405</v>
       </c>
     </row>
@@ -19597,31 +21401,31 @@
         <v>19</v>
       </c>
       <c r="B8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>10</v>
       </c>
       <c r="C8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>8</v>
       </c>
       <c r="D8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>0</v>
       </c>
       <c r="E8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>21</v>
       </c>
       <c r="F8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>2</v>
       </c>
       <c r="G8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>1</v>
       </c>
       <c r="H8" s="59">
-        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$M:$M,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>1</v>
       </c>
     </row>
@@ -19630,31 +21434,31 @@
         <v>20</v>
       </c>
       <c r="B9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>9</v>
       </c>
       <c r="C9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>11</v>
       </c>
       <c r="D9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>11</v>
       </c>
       <c r="E9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>18</v>
       </c>
       <c r="F9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>19</v>
       </c>
       <c r="G9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>30</v>
       </c>
       <c r="H9" s="59">
-        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$N:$N,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>2</v>
       </c>
     </row>
@@ -19663,31 +21467,31 @@
         <v>22</v>
       </c>
       <c r="B10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>1642</v>
       </c>
       <c r="C10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>2173</v>
       </c>
       <c r="D10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>6055</v>
       </c>
       <c r="E10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>863</v>
       </c>
       <c r="F10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>1524</v>
       </c>
       <c r="G10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>7131</v>
       </c>
       <c r="H10" s="59">
-        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$O:$O,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>3258</v>
       </c>
     </row>
@@ -19696,31 +21500,31 @@
         <v>23</v>
       </c>
       <c r="B11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>40</v>
       </c>
       <c r="C11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>71</v>
       </c>
       <c r="D11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>-27</v>
       </c>
       <c r="E11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>-64</v>
       </c>
       <c r="F11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>242</v>
       </c>
       <c r="G11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>109</v>
       </c>
       <c r="H11" s="59">
-        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$P:$P,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>47</v>
       </c>
     </row>
@@ -19729,31 +21533,31 @@
         <v>24</v>
       </c>
       <c r="B12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>15</v>
       </c>
       <c r="C12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>0</v>
       </c>
       <c r="D12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>16</v>
       </c>
       <c r="E12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>0</v>
       </c>
       <c r="F12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>16</v>
       </c>
       <c r="G12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>37</v>
       </c>
       <c r="H12" s="59">
-        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$Q:$Q,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>5</v>
       </c>
     </row>
@@ -19762,31 +21566,31 @@
         <v>25</v>
       </c>
       <c r="B13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>354</v>
       </c>
       <c r="C13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>346</v>
       </c>
       <c r="D13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>-164</v>
       </c>
       <c r="E13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>590</v>
       </c>
       <c r="F13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>2432</v>
       </c>
       <c r="G13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>1123</v>
       </c>
       <c r="H13" s="59">
-        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$R:$R,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>257</v>
       </c>
     </row>
@@ -19795,31 +21599,31 @@
         <v>26</v>
       </c>
       <c r="B14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!B4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!B4),0)</f>
         <v>-756</v>
       </c>
       <c r="C14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!C4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!C4),0)</f>
         <v>2532</v>
       </c>
       <c r="D14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!D4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!D4),0)</f>
         <v>3965</v>
       </c>
       <c r="E14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!E4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!E4),0)</f>
         <v>4794</v>
       </c>
       <c r="F14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!F4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!F4),0)</f>
         <v>6631</v>
       </c>
       <c r="G14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!G4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!G4),0)</f>
         <v>3653</v>
       </c>
       <c r="H14" s="59">
-        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AM:$AM,Weekday!H4),0)</f>
+        <f>IFERROR(SUMIFS(Data!$S:$S,Data!$AN:$AN,Weekday!H4),0)</f>
         <v>-892</v>
       </c>
     </row>
@@ -23670,7 +25474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19627BE-9E30-476B-B050-C456CF349742}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>